<commit_message>
- Updated the Proposal Data logic.
</commit_message>
<xml_diff>
--- a/TIG Project Updated Analysis 06062025/Input/Nick Data/TIG utilization report July 2025.xlsx
+++ b/TIG Project Updated Analysis 06062025/Input/Nick Data/TIG utilization report July 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholasgiraldo/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwy-my.sharepoint.com/personal/mhossa11_uwyo_edu/Documents/Projects/Business Manager Jami Work Requests/TIG Project Updated Analysis 06062025/Input/Nick Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC50337F-0766-0442-9A10-6C3A18D77C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{AC50337F-0766-0442-9A10-6C3A18D77C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{027AFF0E-9C17-406D-B6E9-B4504C265841}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="1980" windowWidth="26040" windowHeight="14940" xr2:uid="{2AC21E09-EAE5-604F-8BE9-8F7D983C22F6}"/>
+    <workbookView xWindow="28680" yWindow="105" windowWidth="29040" windowHeight="15720" xr2:uid="{2AC21E09-EAE5-604F-8BE9-8F7D983C22F6}"/>
   </bookViews>
   <sheets>
     <sheet name="TIG Raw Data" sheetId="1" r:id="rId1"/>
@@ -1163,19 +1163,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B804AC-726D-AB43-A8E9-F264C5F693CC}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="37" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1254,7 +1255,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1286,7 +1287,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1318,7 +1319,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1359,7 +1360,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1400,7 +1401,7 @@
       </c>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1470,7 +1471,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -1546,7 +1547,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1581,7 +1582,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1642,7 +1643,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1721,7 +1722,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -1753,7 +1754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -1791,7 +1792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -1829,7 +1830,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -1861,7 +1862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -1899,7 +1900,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>104</v>
       </c>
@@ -1934,7 +1935,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>119</v>
       </c>
@@ -1969,7 +1970,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>124</v>
       </c>
@@ -2010,7 +2011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2086,7 +2087,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2124,7 +2125,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2235,7 +2236,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -2270,7 +2271,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -2305,7 +2306,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -2340,7 +2341,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -2375,7 +2376,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>90</v>
       </c>
@@ -2448,7 +2449,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>90</v>
       </c>
@@ -2521,7 +2522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -2556,7 +2557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>192</v>
       </c>
@@ -2591,7 +2592,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>192</v>
       </c>
@@ -2629,7 +2630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>192</v>
       </c>
@@ -2664,7 +2665,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -2693,7 +2694,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>124</v>
       </c>
@@ -2725,7 +2726,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>124</v>
       </c>
@@ -2760,7 +2761,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2798,7 +2799,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>14</v>
       </c>
@@ -2839,7 +2840,7 @@
       </c>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2871,7 +2872,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -2906,7 +2907,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -2941,7 +2942,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -2973,7 +2974,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>33</v>
       </c>
@@ -3008,7 +3009,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -3037,7 +3038,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -3075,7 +3076,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -3113,7 +3114,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>72</v>
       </c>

</xml_diff>